<commit_message>
Vanilla Brewing Expanded 업데이트
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Brewing Expanded - 2186560858/2186560858.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Brewing Expanded - 2186560858/2186560858.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Vanilla Brewing Expanded - 2186560858\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Vanilla Expanded\Vanilla Brewing Expanded - 2186560858\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267D6BF0-73D4-4793-A8BB-9621D84D1C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0162F0-2696-4C45-9203-C968F2983B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,6 +493,197 @@
         </r>
       </text>
     </comment>
+    <comment ref="E380" authorId="0" shapeId="0" xr:uid="{8E2D1E73-C1A5-464E-B745-9ED853C8A825}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">{0}: </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>암브랜디</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> label</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E381" authorId="0" shapeId="0" xr:uid="{85175565-7DEF-4F42-9B1D-2A9AD1FB06C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">{0}: </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>암브랜디</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> label
+e.g. </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>암브랜디</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>걸작</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E393" authorId="0" shapeId="0" xr:uid="{9C05940E-278A-427A-AD6C-050E091C0965}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>얘네</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>어디</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>나오는건지</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>모르겠음</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E404" authorId="0" shapeId="0" xr:uid="{79A5CCC7-4B2A-4EED-B1E6-CBB16275BF74}">
       <text>
         <r>
@@ -780,7 +971,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2914" uniqueCount="1575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2916" uniqueCount="1582">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -5587,6 +5778,34 @@
   </si>
   <si>
     <t>소다 주입기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gizmo Label</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gizmo Desc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0} 추출</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>증류를 끝내고 {0}(을)를 증류기에서 {0}(을)를 추출합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>남은 숙성 시간: {0} (냉장되어 느려짐)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>남은 숙성 시간: 냉동되어 중단됨</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>남은 숙성 시간: {0}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -5760,7 +5979,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -5773,9 +5992,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="3" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="메모" xfId="2" builtinId="10"/>
@@ -6083,8 +6303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G416"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E410" sqref="E410"/>
+    <sheetView tabSelected="1" topLeftCell="B370" workbookViewId="0">
+      <selection activeCell="E406" sqref="E406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -14109,8 +14329,11 @@
       <c r="D380" s="1" t="s">
         <v>1082</v>
       </c>
-      <c r="E380" s="1" t="s">
-        <v>1196</v>
+      <c r="E380" s="11" t="s">
+        <v>1577</v>
+      </c>
+      <c r="F380" s="1" t="s">
+        <v>1575</v>
       </c>
       <c r="G380" t="str">
         <f>IFERROR(VLOOKUP(A380,Merge!$C$2:$D$410,2,FALSE),"")</f>
@@ -14130,8 +14353,11 @@
       <c r="D381" s="5" t="s">
         <v>1085</v>
       </c>
-      <c r="E381" s="5" t="s">
-        <v>1197</v>
+      <c r="E381" s="15" t="s">
+        <v>1578</v>
+      </c>
+      <c r="F381" s="14" t="s">
+        <v>1576</v>
       </c>
       <c r="G381" t="str">
         <f>IFERROR(VLOOKUP(A381,Merge!$C$2:$D$410,2,FALSE),"")</f>
@@ -14205,16 +14431,16 @@
       </c>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A385" s="12" t="s">
+      <c r="A385" s="1" t="s">
         <v>1095</v>
       </c>
-      <c r="B385" s="12" t="s">
+      <c r="B385" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="C385" s="12" t="s">
+      <c r="C385" s="1" t="s">
         <v>1560</v>
       </c>
-      <c r="D385" s="12" t="s">
+      <c r="D385" s="1" t="s">
         <v>1096</v>
       </c>
       <c r="E385" s="10" t="s">
@@ -14239,7 +14465,7 @@
         <v>1561</v>
       </c>
       <c r="D386" s="5"/>
-      <c r="E386" s="14" t="s">
+      <c r="E386" s="13" t="s">
         <v>1562</v>
       </c>
       <c r="F386" s="8"/>
@@ -14347,7 +14573,7 @@
       <c r="D391" s="5" t="s">
         <v>1108</v>
       </c>
-      <c r="E391" s="14" t="s">
+      <c r="E391" s="13" t="s">
         <v>1562</v>
       </c>
       <c r="F391" s="8" t="s">
@@ -14461,7 +14687,7 @@
       <c r="D396" s="5" t="s">
         <v>1123</v>
       </c>
-      <c r="E396" s="14" t="s">
+      <c r="E396" s="13" t="s">
         <v>1562</v>
       </c>
       <c r="F396" s="8" t="s">
@@ -14575,7 +14801,7 @@
       <c r="D401" s="5" t="s">
         <v>1138</v>
       </c>
-      <c r="E401" s="14" t="s">
+      <c r="E401" s="13" t="s">
         <v>1562</v>
       </c>
       <c r="F401" s="8" t="s">
@@ -14602,7 +14828,7 @@
       <c r="E402" s="10" t="s">
         <v>1565</v>
       </c>
-      <c r="F402" s="13" t="s">
+      <c r="F402" s="12" t="s">
         <v>1564</v>
       </c>
       <c r="G402" t="str">
@@ -14708,7 +14934,7 @@
         <v>1156</v>
       </c>
       <c r="E407" s="1" t="s">
-        <v>1205</v>
+        <v>1580</v>
       </c>
       <c r="G407" t="str">
         <f>IFERROR(VLOOKUP(A407,Merge!$C$2:$D$410,2,FALSE),"")</f>
@@ -14729,7 +14955,7 @@
         <v>1159</v>
       </c>
       <c r="E408" s="1" t="s">
-        <v>1206</v>
+        <v>1579</v>
       </c>
       <c r="G408" t="str">
         <f>IFERROR(VLOOKUP(A408,Merge!$C$2:$D$410,2,FALSE),"")</f>
@@ -14750,7 +14976,7 @@
         <v>1162</v>
       </c>
       <c r="E409" s="5" t="s">
-        <v>1207</v>
+        <v>1581</v>
       </c>
       <c r="G409" t="str">
         <f>IFERROR(VLOOKUP(A409,Merge!$C$2:$D$410,2,FALSE),"")</f>

</xml_diff>